<commit_message>
Create new GGSlides for WrapUp presentation
</commit_message>
<xml_diff>
--- a/Presentation/Presentation-Graph_example.xlsx
+++ b/Presentation/Presentation-Graph_example.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trang\Google Drive\UQAM\Courses\BIO6065_ET20\DDES-GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trang\Google Drive\UQAM\Courses\BIO6065_ET20\DDES-GitHub\VirtualBiogeography\Presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B054ABA9-3E20-4C04-9E4F-26E0CB8A3271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5D70BC-4412-41C6-B7F2-00DAB4330F55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10160" yWindow="210" windowWidth="8840" windowHeight="7360" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TotalV.Unidentifiable" sheetId="2" r:id="rId1"/>
     <sheet name="TotalV.Indentifiable" sheetId="3" r:id="rId2"/>
     <sheet name="example-data" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
   <si>
     <t>screenshot_#</t>
   </si>
@@ -47,6 +48,531 @@
   </si>
   <si>
     <t>Identifiable</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>SS_00-01-04_GBR.png</t>
+  </si>
+  <si>
+    <t>SS_00-01-12_GBR.png</t>
+  </si>
+  <si>
+    <t>SS_00-01-30_GBR.png</t>
+  </si>
+  <si>
+    <t>SS_00-01-31_GBR.png</t>
+  </si>
+  <si>
+    <t>SS_00-01-33_GBR.png</t>
+  </si>
+  <si>
+    <t>SS_00-01-34_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-01-36_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-01-37_GBR.png</t>
+  </si>
+  <si>
+    <t>SS_00-01-48_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-02-05_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-02-08_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-02-16_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-02-44_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-03-04_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-03-13_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-05-28_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-05-34_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-05-42_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-05-53_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-06-47_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-18_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-26_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-35_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-40_GBR(2).PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-40_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-41_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-43_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-49_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-51_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-53_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-56_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-07-58_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-08-01_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-08-03_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-08-04_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-08-09_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-08-12_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-08-53_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-09-02_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-09-47_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-09-54_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-09-57_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-10-02_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-10-08_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-10-13_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-10-20_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-10-39_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-10-42_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-10-43_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-10-47_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-18_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-20_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-21_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-22_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-24_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-27_GBR(2).PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-27_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-28_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-29_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-31_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-32_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-33_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-36_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-38_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-40_GBR(2).PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-40_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-42_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-43_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-44_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-47_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-49_GBR(2).PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-49_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-50_GBR(2).PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-50_GBR(3).PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-50_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-11-52_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-12-02_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-12-21_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-12-23_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-13-43_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-14-05_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-15-08_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-33_SPO(2).PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-33_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-34_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-35_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-37_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-39_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-40_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-46_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-48_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-16-58_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-17-02_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-17-05_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-17-09_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-17-11_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-17-14_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-17-34_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-17-37_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-19-00_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-20-34_SL.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-20-52_SL.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-21-05_SL.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-22-55_SL.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-25-26_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-26-48_DO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-26-55_DO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-27-18_DO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-27-51_DO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-28-32_DO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-28-54_DO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-29-50_DO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-34-13_T.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-40-37_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-40-43_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-40-54_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-41-57_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-45-53_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-45-55_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-51-47_EAC.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-52-36_EAC.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-52-42_EAC.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-52-50_EAC.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-54-00_EAC.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-55-38_EAC.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-56-33_EAC.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-56-38_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-56-44_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-56-52_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-56-58_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-57-00_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-57-02_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-57-05_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-57-08_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-57-25_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-57-27_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-57-34_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-57-44_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_00-59-45_DO.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-06-51_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-08-36_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-08-39_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-08-44_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-08-46_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-08-55_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-13-48_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-16-48_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-17-34_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-21-50_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-24-02_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-24-18_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-24-30_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-25-16_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-25-19_FG.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-26-22_FG.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-26-35_FG.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-31-00_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-31-02_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-31-05_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-31-06_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-31-16_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-31-20_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-31-45_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-31-49_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-31-51_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-32-06_GBR.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-33-20_SH.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-33-36_SPO.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-39-37_credit_MikeWazowski.PNG</t>
+  </si>
+  <si>
+    <t>SS_01-40-12_credit_T.PNG</t>
+  </si>
+  <si>
+    <t>new_identified</t>
+  </si>
+  <si>
+    <t>new_unidentified</t>
+  </si>
+  <si>
+    <t>total_identified</t>
+  </si>
+  <si>
+    <t>total_unidentified-upt</t>
   </si>
 </sst>
 </file>
@@ -4019,7 +4545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+    <sheetView zoomScale="67" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -4498,4 +5024,889 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74238123-9F9F-4401-AD95-B4F002078386}">
+  <dimension ref="A1:E171"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>